<commit_message>
Testing for pull request
</commit_message>
<xml_diff>
--- a/Assets/Resources/Excel Sheets/Straatroof.xlsx
+++ b/Assets/Resources/Excel Sheets/Straatroof.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\BartVR\Assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_BartVR\Assets\Resources\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258CA2A8-0749-4324-91AF-B591CB5F33A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F92684-D9DD-4C5B-9802-F66EC249EDDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{78A6683D-15A0-4C0D-8F6C-014DD2D0FE0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -179,9 +179,6 @@
     <t>Heeft iemand de overvaller gezien?</t>
   </si>
   <si>
-    <t>Een man stal een tas van een vrouw.</t>
-  </si>
-  <si>
     <t>Schokkend dat het gebeurt op klaarlichte dag.</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Is de verdachte gevaarlijk?</t>
   </si>
   <si>
-    <t>Ik zag iemand hier wegrennen met een tas!</t>
-  </si>
-  <si>
     <t>Tas was hier gedumpt, heb het naar de politie gebracht.</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>Is dit al opgelost?</t>
   </si>
   <si>
-    <t>De persoon die de tas dumpte had een zwart shirt aan.</t>
-  </si>
-  <si>
     <t>Ik zag de overval voor mijn ogen gebeuren.</t>
   </si>
   <si>
@@ -218,15 +209,9 @@
     <t>Was de verdachte een vrouw?</t>
   </si>
   <si>
-    <t>De man rende hier gauw weg!</t>
-  </si>
-  <si>
     <t>Hoe ziet de verdachte eruit?</t>
   </si>
   <si>
-    <t>De overvaller loopt hier volgens mij.</t>
-  </si>
-  <si>
     <t>Ik zie een uitgeput persoon hier van het rennen.</t>
   </si>
   <si>
@@ -318,6 +303,21 @@
   </si>
   <si>
     <t>Postable</t>
+  </si>
+  <si>
+    <t>Een [geslacht] stal een tas van een vrouw.</t>
+  </si>
+  <si>
+    <t>De[geslacht] rende hier gauw weg!</t>
+  </si>
+  <si>
+    <t>Ik zag iemand hier wegrennen met een tas en een [bovenstuk] bovenstuk!</t>
+  </si>
+  <si>
+    <t>De persoon die de tas dumpte had een [bovenstuk] shirt aan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De overvaller loopt hier volgens mij. De [geslacht] draagt een [onderstuk] onderstuk! </t>
   </si>
 </sst>
 </file>
@@ -417,6 +417,10 @@
   <dxfs count="3">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -461,80 +465,8 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -587,7 +519,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{130B8255-2A90-4E8D-A984-0435A7EE0031}" name="Tabel2" displayName="Tabel2" ref="A1:G24" tableType="xml" totalsRowShown="0" connectionId="3">
   <autoFilter ref="A1:G24" xr:uid="{C46271E9-EE0C-40FA-9CDC-770352DE17CB}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{E954BD75-C2AF-4AB0-A020-84687C11D4B3}" uniqueName="Id" name="Id" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{E954BD75-C2AF-4AB0-A020-84687C11D4B3}" uniqueName="Id" name="Id" dataDxfId="2">
       <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Id" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{5566690A-8CE2-4A65-84CB-742B8A242D2A}" uniqueName="ReactionTo" name="ReactionTo" dataDxfId="1">
@@ -599,7 +531,7 @@
     <tableColumn id="3" xr3:uid="{A638FCF3-299C-43A1-B5FE-6EE0A4E20EB4}" uniqueName="Message" name="Message">
       <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Message" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="Image" name="Image" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{04887506-595B-46D5-8C69-7E2023ED2F8F}" uniqueName="Image" name="Image" dataDxfId="0">
       <xmlColumnPr mapId="12" xpath="/NotificationCollection/Notifications/Notification/Image" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{16A70CAA-E4E0-4408-9EEC-8CB58EC31095}" uniqueName="Platform" name="Platform">
@@ -618,7 +550,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="040404"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -913,7 +845,7 @@
   <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,13 +860,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -946,12 +878,12 @@
         <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="2" t="s">
@@ -970,16 +902,16 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>19</v>
@@ -993,10 +925,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>27</v>
@@ -1009,12 +941,12 @@
         <v>2</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
@@ -1033,14 +965,14 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1052,14 +984,14 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1072,14 +1004,14 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
@@ -1091,14 +1023,14 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
@@ -1110,14 +1042,14 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
@@ -1129,14 +1061,14 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
@@ -1148,14 +1080,14 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
@@ -1167,16 +1099,16 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1188,14 +1120,14 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1207,14 +1139,14 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1226,14 +1158,14 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
@@ -1245,14 +1177,14 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1264,14 +1196,14 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
@@ -1283,14 +1215,14 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
@@ -1302,17 +1234,17 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>2</v>
@@ -1323,14 +1255,14 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
@@ -1344,16 +1276,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
@@ -1365,7 +1297,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="2" t="s">
@@ -1386,14 +1318,14 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">

</xml_diff>